<commit_message>
FIGS: tikzpicture, figured out how to create figs
</commit_message>
<xml_diff>
--- a/ABIP.xlsx
+++ b/ABIP.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Ex 5.3" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Dt</t>
   </si>
@@ -43,6 +44,27 @@
   </si>
   <si>
     <t>xi</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>start angle</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>end angle</t>
   </si>
 </sst>
 </file>
@@ -1145,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1191,11 +1213,11 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <f>B3*12*2.54/100</f>
+        <f t="shared" ref="D3:E7" si="0">B3*12*2.54/100</f>
         <v>3.6576</v>
       </c>
       <c r="E3">
-        <f>C3*12*2.54/100</f>
+        <f t="shared" si="0"/>
         <v>2.7431999999999999</v>
       </c>
       <c r="F3">
@@ -1231,11 +1253,11 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <f>B4*12*2.54/100</f>
+        <f t="shared" si="0"/>
         <v>3.6576</v>
       </c>
       <c r="E4">
-        <f>C4*12*2.54/100</f>
+        <f t="shared" si="0"/>
         <v>1.8288</v>
       </c>
       <c r="F4">
@@ -1271,11 +1293,11 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <f>B5*12*2.54/100</f>
+        <f t="shared" si="0"/>
         <v>3.6576</v>
       </c>
       <c r="E5">
-        <f>C5*12*2.54/100</f>
+        <f t="shared" si="0"/>
         <v>0.30480000000000002</v>
       </c>
       <c r="F5">
@@ -1311,11 +1333,11 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f>B6*12*2.54/100</f>
+        <f t="shared" si="0"/>
         <v>3.6576</v>
       </c>
       <c r="E6">
-        <f>C6*12*2.54/100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6">
@@ -1351,11 +1373,11 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <f>B7*12*2.54/100</f>
+        <f t="shared" si="0"/>
         <v>2.4384000000000001</v>
       </c>
       <c r="E7">
-        <f>C7*12*2.54/100</f>
+        <f t="shared" si="0"/>
         <v>1.524</v>
       </c>
       <c r="F7">
@@ -1386,4 +1408,2585 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:V40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.26953125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="47.54296875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="6.26953125" hidden="1" customWidth="1"/>
+    <col min="13" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="43" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="90.453125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="92.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="R1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="R2">
+        <v>9</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>10</v>
+      </c>
+      <c r="U2">
+        <f>90+ATAN(-(R40-R4)/(S40-S4))/PI()*180</f>
+        <v>51.366666116958356</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="R3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <f>R2-T4*COS(T2/180*PI())</f>
+        <v>-7.7417318012075356</v>
+      </c>
+      <c r="S4">
+        <f>S2+T4*SIN(T2/180*PI())</f>
+        <v>3.9520190203378158</v>
+      </c>
+      <c r="T4">
+        <v>17</v>
+      </c>
+      <c r="V4" t="str">
+        <f>CONCATENATE("\draw [lightgray] (",R2,",",S2,") arc [radius=",T4,", start angle=-",T2,", end angle=",ROUND(U2+1,0),"];")</f>
+        <v>\draw [lightgray] (9,1) arc [radius=17, start angle=-10, end angle=52];</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C40" si="0">(B5-D5+1)/6+1</f>
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D40" si="1">MOD(B5,6)+1</f>
+        <v>1</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" ref="E5:E40" si="2">CONCATENATE("\draw [-&gt;] (",C5,",",D5,")")</f>
+        <v>\draw [-&gt;] (6,1)</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G40" si="3">SQRT(C5^2+D5^2)</f>
+        <v>6.0827625302982193</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H40" si="4">C5*$G$4/$G5</f>
+        <v>5.9183635429928625</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I40" si="5">D5*$G$4/$G5</f>
+        <v>0.98639392383214375</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" ref="J5:J40" si="6">CONCATENATE("\draw [-&gt;] (0,0) -- (",ROUND(H5,2),",",ROUND(I5,2),"); ","\draw (0,0) -- (",ROUND(M5,2),",",ROUND(N5,2),"); ")</f>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.92,0.99); \draw (0,0) -- (7.89,1.32); </v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L40" si="7">SQRT(C5^2+D5^2)</f>
+        <v>6.0827625302982193</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M40" si="8">C5*$L$4/$L5</f>
+        <v>7.89115139065715</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N40" si="9">D5*$L$4/$L5</f>
+        <v>1.3151918984428583</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O40" si="10">ATAN(D5/C5)/PI()*180</f>
+        <v>9.4623222080256184</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" ref="P5:P40" si="11">CONCATENATE("\node [",IF(O5&lt;20,"below right",IF(O5&lt;35,"right",IF(O5&lt;55,"above right",IF(O5&lt;70,"above","above left")))),"] at (",ROUND(M5,2),",",ROUND(N5,2),") {$",ROUND(O5,2),"^\circ$};")</f>
+        <v>\node [below right] at (7.89,1.32) {$9.46^\circ$};</v>
+      </c>
+      <c r="Q5" t="str">
+        <f>CONCATENATE(IF(O5=O4,"% ",""),"\draw [-&gt;] (0,0) -- (",ROUND(H5,2),",",ROUND(I5,2),"); \draw (0,0) -- (",ROUND(IF(O5&lt;45,50,IF(O5&lt;60,30,22))/(5+D5/C5),2),",",ROUND(IF(O5&lt;45,50,IF(O5&lt;60,30,22))*D5/(5*C5+D5),2),");  \node [right] at (",ROUND(IF(O5&lt;45,50,IF(O5&lt;60,30,22))/(5+D5/C5),2),",",ROUND(IF(O5&lt;45,50,IF(O5&lt;60,30,22))*D5/(5*C5+D5),2),") {(",C5,",",D5,") $",ROUND(O5,2),"^\circ$};")</f>
+        <v>\draw [-&gt;] (0,0) -- (5.92,0.99); \draw (0,0) -- (9.68,1.61);  \node [right] at (9.68,1.61) {(6,1) $9.46^\circ$};</v>
+      </c>
+      <c r="R5">
+        <f>(2*($R$4+D5/C5*$S$4)+2*SQRT(($R$4+D5/C5*$S$4)^2-(1+(D5/C5)^2)*($R$4^2+$S$4^2-$T$4^2)))/(2*(1+(D5/C5)^2))</f>
+        <v>9.082502085646972</v>
+      </c>
+      <c r="S5">
+        <f>R5*D5/C5</f>
+        <v>1.5137503476078287</v>
+      </c>
+      <c r="V5" t="str">
+        <f>CONCATENATE(IF(O5=O4,"% ",""),"\draw [-&gt;] (0,0) -- (",ROUND(H5,2),",",ROUND(I5,2),"); \draw (0,0) -- (",ROUND(R5,2),",",ROUND(S5,2),");  \node [right] at (",ROUND(R5,2),",",ROUND(S5,2),") {(",C5,",",D5,") $",ROUND(O5,2),"^\circ$};")</f>
+        <v>\draw [-&gt;] (0,0) -- (5.92,0.99); \draw (0,0) -- (9.08,1.51);  \node [right] at (9.08,1.51) {(6,1) $9.46^\circ$};</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (5,1)</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>5.8834840541455211</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="5"/>
+        <v>1.1766968108291043</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.88,1.18); \draw (0,0) -- (7.84,1.57); </v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="7"/>
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="8"/>
+        <v>7.8446454055273618</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="9"/>
+        <v>1.5689290811054724</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="10"/>
+        <v>11.309932474020215</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [below right] at (7.84,1.57) {$11.31^\circ$};</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" ref="Q6:Q40" si="12">CONCATENATE(IF(O6=O5,"% ",""),"\draw [-&gt;] (0,0) -- (",ROUND(H6,2),",",ROUND(I6,2),"); \draw (0,0) -- (",ROUND(IF(O6&lt;45,50,IF(O6&lt;60,30,22))/(5+D6/C6),2),",",ROUND(IF(O6&lt;45,50,IF(O6&lt;60,30,22))*D6/(5*C6+D6),2),");  \node [right] at (",ROUND(IF(O6&lt;45,50,IF(O6&lt;60,30,22))/(5+D6/C6),2),",",ROUND(IF(O6&lt;45,50,IF(O6&lt;60,30,22))*D6/(5*C6+D6),2),") {(",C6,",",D6,") $",ROUND(O6,2),"^\circ$};")</f>
+        <v>\draw [-&gt;] (0,0) -- (5.88,1.18); \draw (0,0) -- (9.62,1.92);  \node [right] at (9.62,1.92) {(5,1) $11.31^\circ$};</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R40" si="13">(2*($R$4+D6/C6*$S$4)+2*SQRT(($R$4+D6/C6*$S$4)^2-(1+(D6/C6)^2)*($R$4^2+$S$4^2-$T$4^2)))/(2*(1+(D6/C6)^2))</f>
+        <v>9.1246699877281561</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:S40" si="14">R6*D6/C6</f>
+        <v>1.8249339975456311</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" ref="V6:V40" si="15">CONCATENATE(IF(O6=O5,"% ",""),"\draw [-&gt;] (0,0) -- (",ROUND(H6,2),",",ROUND(I6,2),"); \draw (0,0) -- (",ROUND(R6,2),",",ROUND(S6,2),");  \node [right] at (",ROUND(R6,2),",",ROUND(S6,2),") {(",C6,",",D6,") $",ROUND(O6,2),"^\circ$};")</f>
+        <v>\draw [-&gt;] (0,0) -- (5.88,1.18); \draw (0,0) -- (9.12,1.82);  \node [right] at (9.12,1.82) {(5,1) $11.31^\circ$};</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (4,1)</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>4.1231056256176606</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>5.8208550008719913</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="5"/>
+        <v>1.4552137502179978</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.82,1.46); \draw (0,0) -- (7.76,1.94); </v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="7"/>
+        <v>4.1231056256176606</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="8"/>
+        <v>7.761140001162655</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="9"/>
+        <v>1.9402850002906638</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="10"/>
+        <v>14.036243467926479</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [below right] at (7.76,1.94) {$14.04^\circ$};</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (5.82,1.46); \draw (0,0) -- (9.52,2.38);  \node [right] at (9.52,2.38) {(4,1) $14.04^\circ$};</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="13"/>
+        <v>9.1772519359150575</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="14"/>
+        <v>2.2943129839787644</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (5.82,1.46); \draw (0,0) -- (9.18,2.29);  \node [right] at (9.18,2.29) {(4,1) $14.04^\circ$};</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (3,1)</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>5.6920997883030822</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>1.8973665961010275</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.69,1.9); \draw (0,0) -- (7.59,2.53); </v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="7"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="8"/>
+        <v>7.5894663844041101</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="9"/>
+        <v>2.5298221281347035</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="10"/>
+        <v>18.43494882292201</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [below right] at (7.59,2.53) {$18.43^\circ$};</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (5.69,1.9); \draw (0,0) -- (9.38,3.13);  \node [right] at (9.38,3.13) {(3,1) $18.43^\circ$};</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="13"/>
+        <v>9.2358165749908494</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="14"/>
+        <v>3.0786055249969499</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (5.69,1.9); \draw (0,0) -- (9.24,3.08);  \node [right] at (9.24,3.08) {(3,1) $18.43^\circ$};</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (6,2)</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>6.324555320336759</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>5.6920997883030822</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>1.8973665961010275</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.69,1.9); \draw (0,0) -- (7.59,2.53); </v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="7"/>
+        <v>6.324555320336759</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="8"/>
+        <v>7.5894663844041101</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="9"/>
+        <v>2.5298221281347035</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="10"/>
+        <v>18.43494882292201</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [below right] at (7.59,2.53) {$18.43^\circ$};</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (5.69,1.9); \draw (0,0) -- (9.38,3.13);  \node [right] at (9.38,3.13) {(6,2) $18.43^\circ$};</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="13"/>
+        <v>9.2358165749908494</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="14"/>
+        <v>3.0786055249969499</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (5.69,1.9); \draw (0,0) -- (9.24,3.08);  \node [right] at (9.24,3.08) {(6,2) $18.43^\circ$};</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (5,2)</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>5.3851648071345037</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>5.5708601453115563</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>2.2283440581246223</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.57,2.23); \draw (0,0) -- (7.43,2.97); </v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="7"/>
+        <v>5.3851648071345037</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="8"/>
+        <v>7.4278135270820753</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="9"/>
+        <v>2.9711254108328298</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="10"/>
+        <v>21.801409486351815</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [right] at (7.43,2.97) {$21.8^\circ$};</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (5.57,2.23); \draw (0,0) -- (9.26,3.7);  \node [right] at (9.26,3.7) {(5,2) $21.8^\circ$};</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="13"/>
+        <v>9.2564380352048712</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="14"/>
+        <v>3.7025752140819486</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (5.57,2.23); \draw (0,0) -- (9.26,3.7);  \node [right] at (9.26,3.7) {(5,2) $21.8^\circ$};</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (2,1)</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>5.3665631459994954</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>2.6832815729997477</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.37,2.68); \draw (0,0) -- (7.16,3.58); </v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="7"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="8"/>
+        <v>7.1554175279993268</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="9"/>
+        <v>3.5777087639996634</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="10"/>
+        <v>26.565051177077986</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [right] at (7.16,3.58) {$26.57^\circ$};</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (5.37,2.68); \draw (0,0) -- (9.09,4.55);  \node [right] at (9.09,4.55) {(2,1) $26.57^\circ$};</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="13"/>
+        <v>9.2450403524407303</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="14"/>
+        <v>4.6225201762203652</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (5.37,2.68); \draw (0,0) -- (9.25,4.62);  \node [right] at (9.25,4.62) {(2,1) $26.57^\circ$};</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (4,2)</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>5.3665631459994954</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>2.6832815729997477</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.37,2.68); \draw (0,0) -- (7.16,3.58); </v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="7"/>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="8"/>
+        <v>7.1554175279993268</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="9"/>
+        <v>3.5777087639996634</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="10"/>
+        <v>26.565051177077986</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [right] at (7.16,3.58) {$26.57^\circ$};</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (5.37,2.68); \draw (0,0) -- (9.09,4.55);  \node [right] at (9.09,4.55) {(4,2) $26.57^\circ$};</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="13"/>
+        <v>9.2450403524407303</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="14"/>
+        <v>4.6225201762203652</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (5.37,2.68); \draw (0,0) -- (9.25,4.62);  \node [right] at (9.25,4.62) {(4,2) $26.57^\circ$};</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (6,3)</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>6.7082039324993694</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>5.3665631459994954</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>2.6832815729997477</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.37,2.68); \draw (0,0) -- (7.16,3.58); </v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="7"/>
+        <v>6.7082039324993694</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="8"/>
+        <v>7.1554175279993268</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="9"/>
+        <v>3.5777087639996634</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="10"/>
+        <v>26.565051177077986</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [right] at (7.16,3.58) {$26.57^\circ$};</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (5.37,2.68); \draw (0,0) -- (9.09,4.55);  \node [right] at (9.09,4.55) {(6,3) $26.57^\circ$};</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="13"/>
+        <v>9.2450403524407303</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="14"/>
+        <v>4.6225201762203652</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (5.37,2.68); \draw (0,0) -- (9.25,4.62);  \node [right] at (9.25,4.62) {(6,3) $26.57^\circ$};</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (5,3)</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>5.8309518948453007</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>5.1449575542752646</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>3.0869745325651587</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (5.14,3.09); \draw (0,0) -- (6.86,4.12); </v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="7"/>
+        <v>5.8309518948453007</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="8"/>
+        <v>6.8599434057003528</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="9"/>
+        <v>4.1159660434202117</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="10"/>
+        <v>30.963756532073525</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [right] at (6.86,4.12) {$30.96^\circ$};</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (5.14,3.09); \draw (0,0) -- (8.93,5.36);  \node [right] at (8.93,5.36) {(5,3) $30.96^\circ$};</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="13"/>
+        <v>9.1865486843661497</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="14"/>
+        <v>5.5119292106196891</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (5.14,3.09); \draw (0,0) -- (9.19,5.51);  \node [right] at (9.19,5.51) {(5,3) $30.96^\circ$};</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (3,2)</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>4.9923017660270625</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>3.3282011773513749</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.99,3.33); \draw (0,0) -- (6.66,4.44); </v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="7"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="8"/>
+        <v>6.6564023547027498</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="9"/>
+        <v>4.4376015698018332</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="10"/>
+        <v>33.690067525979785</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [right] at (6.66,4.44) {$33.69^\circ$};</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (4.99,3.33); \draw (0,0) -- (8.82,5.88);  \node [right] at (8.82,5.88) {(3,2) $33.69^\circ$};</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="13"/>
+        <v>9.1242031961833963</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="14"/>
+        <v>6.0828021307889308</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (4.99,3.33); \draw (0,0) -- (9.12,6.08);  \node [right] at (9.12,6.08) {(3,2) $33.69^\circ$};</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (6,4)</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>4.9923017660270625</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>3.3282011773513749</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.99,3.33); \draw (0,0) -- (6.66,4.44); </v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="7"/>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="8"/>
+        <v>6.6564023547027498</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="9"/>
+        <v>4.4376015698018332</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="10"/>
+        <v>33.690067525979785</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [right] at (6.66,4.44) {$33.69^\circ$};</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.99,3.33); \draw (0,0) -- (8.82,5.88);  \node [right] at (8.82,5.88) {(6,4) $33.69^\circ$};</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="13"/>
+        <v>9.1242031961833963</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="14"/>
+        <v>6.0828021307889308</v>
+      </c>
+      <c r="V16" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.99,3.33); \draw (0,0) -- (9.12,6.08);  \node [right] at (9.12,6.08) {(6,4) $33.69^\circ$};</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (4,3)</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>4.8</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>3.6</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.8,3.6); \draw (0,0) -- (6.4,4.8); </v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="8"/>
+        <v>6.4</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="9"/>
+        <v>4.8</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="10"/>
+        <v>36.86989764584402</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (6.4,4.8) {$36.87^\circ$};</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (4.8,3.6); \draw (0,0) -- (8.7,6.52);  \node [right] at (8.7,6.52) {(4,3) $36.87^\circ$};</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="13"/>
+        <v>9.0234831969192051</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="14"/>
+        <v>6.7676123976894038</v>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (4.8,3.6); \draw (0,0) -- (9.02,6.77);  \node [right] at (9.02,6.77) {(4,3) $36.87^\circ$};</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (5,4)</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>6.4031242374328485</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>4.6852128566581817</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>3.7481702853265455</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.69,3.75); \draw (0,0) -- (6.25,5); </v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="7"/>
+        <v>6.4031242374328485</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="8"/>
+        <v>6.2469504755442431</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="9"/>
+        <v>4.9975603804353943</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="10"/>
+        <v>38.659808254090095</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (6.25,5) {$38.66^\circ$};</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (4.69,3.75); \draw (0,0) -- (8.62,6.9);  \node [right] at (8.62,6.9) {(5,4) $38.66^\circ$};</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="13"/>
+        <v>8.9524648710141985</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="14"/>
+        <v>7.1619718968113588</v>
+      </c>
+      <c r="V18" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (4.69,3.75); \draw (0,0) -- (8.95,7.16);  \node [right] at (8.95,7.16) {(5,4) $38.66^\circ$};</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (6,5)</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>7.810249675906654</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="4"/>
+        <v>4.6093276775842549</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="5"/>
+        <v>3.8411063979868794</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.61,3.84); \draw (0,0) -- (6.15,5.12); </v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="7"/>
+        <v>7.810249675906654</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="8"/>
+        <v>6.1457702367790068</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="9"/>
+        <v>5.1214751973158394</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="10"/>
+        <v>39.805571092265197</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (6.15,5.12) {$39.81^\circ$};</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (4.61,3.84); \draw (0,0) -- (8.57,7.14);  \node [right] at (8.57,7.14) {(6,5) $39.81^\circ$};</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="13"/>
+        <v>8.9012539514103892</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="14"/>
+        <v>7.4177116261753246</v>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (4.61,3.84); \draw (0,0) -- (8.9,7.42);  \node [right] at (8.9,7.42) {(6,5) $39.81^\circ$};</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (1,1)</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="5"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5.66,5.66); </v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="7"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="8"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="9"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (5.66,5.66) {$45^\circ$};</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5,5);  \node [right] at (5,5) {(1,1) $45^\circ$};</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="13"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="14"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (8.61,8.61);  \node [right] at (8.61,8.61) {(1,1) $45^\circ$};</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (2,2)</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="5"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5.66,5.66); </v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="7"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="8"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="9"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (5.66,5.66) {$45^\circ$};</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5,5);  \node [right] at (5,5) {(2,2) $45^\circ$};</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="13"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="14"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="V21" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (8.61,8.61);  \node [right] at (8.61,8.61) {(2,2) $45^\circ$};</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (3,3)</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>4.2426406871192857</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="5"/>
+        <v>4.2426406871192857</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5.66,5.66); </v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="7"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="8"/>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="9"/>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (5.66,5.66) {$45^\circ$};</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5,5);  \node [right] at (5,5) {(3,3) $45^\circ$};</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="13"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="14"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="V22" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (8.61,8.61);  \node [right] at (8.61,8.61) {(3,3) $45^\circ$};</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (4,4)</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="5"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5.66,5.66); </v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="7"/>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="8"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="9"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (5.66,5.66) {$45^\circ$};</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5,5);  \node [right] at (5,5) {(4,4) $45^\circ$};</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="13"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="14"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (8.61,8.61);  \node [right] at (8.61,8.61) {(4,4) $45^\circ$};</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>28</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (5,5)</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>7.0710678118654755</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="5"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5.66,5.66); </v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="7"/>
+        <v>7.0710678118654755</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="8"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="9"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (5.66,5.66) {$45^\circ$};</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5,5);  \node [right] at (5,5) {(5,5) $45^\circ$};</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="13"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="14"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (8.61,8.61);  \node [right] at (8.61,8.61) {(5,5) $45^\circ$};</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (6,6)</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>8.4852813742385695</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>4.2426406871192857</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="5"/>
+        <v>4.2426406871192857</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5.66,5.66); </v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="7"/>
+        <v>8.4852813742385695</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="8"/>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="9"/>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="10"/>
+        <v>45</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (5.66,5.66) {$45^\circ$};</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (5,5);  \node [right] at (5,5) {(6,6) $45^\circ$};</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="13"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="14"/>
+        <v>8.6081930682176999</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (4.24,4.24); \draw (0,0) -- (8.61,8.61);  \node [right] at (8.61,8.61) {(6,6) $45^\circ$};</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>29</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (5,6)</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>7.810249675906654</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>3.8411063979868794</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="5"/>
+        <v>4.6093276775842549</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (3.84,4.61); \draw (0,0) -- (5.12,6.15); </v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="7"/>
+        <v>7.810249675906654</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="8"/>
+        <v>5.1214751973158394</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="9"/>
+        <v>6.1457702367790068</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="10"/>
+        <v>50.194428907734803</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (5.12,6.15) {$50.19^\circ$};</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (3.84,4.61); \draw (0,0) -- (4.84,5.81);  \node [right] at (4.84,5.81) {(5,6) $50.19^\circ$};</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="13"/>
+        <v>8.2041905012569103</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="14"/>
+        <v>9.8450286015082931</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (3.84,4.61); \draw (0,0) -- (8.2,9.85);  \node [right] at (8.2,9.85) {(5,6) $50.19^\circ$};</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (4,5)</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>6.4031242374328485</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="4"/>
+        <v>3.7481702853265455</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="5"/>
+        <v>4.6852128566581817</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (3.75,4.69); \draw (0,0) -- (5,6.25); </v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="7"/>
+        <v>6.4031242374328485</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="8"/>
+        <v>4.9975603804353943</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="9"/>
+        <v>6.2469504755442431</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="10"/>
+        <v>51.340191745909905</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (5,6.25) {$51.34^\circ$};</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (3.75,4.69); \draw (0,0) -- (4.8,6);  \node [right] at (4.8,6) {(4,5) $51.34^\circ$};</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="13"/>
+        <v>8.0985956828237757</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="14"/>
+        <v>10.12324460352972</v>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (3.75,4.69); \draw (0,0) -- (8.1,10.12);  \node [right] at (8.1,10.12) {(4,5) $51.34^\circ$};</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (3,4)</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>3.6</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="5"/>
+        <v>4.8</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (3.6,4.8); \draw (0,0) -- (4.8,6.4); </v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="8"/>
+        <v>4.8</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="9"/>
+        <v>6.4</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="10"/>
+        <v>53.130102354155973</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above right] at (4.8,6.4) {$53.13^\circ$};</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (3.6,4.8); \draw (0,0) -- (4.74,6.32);  \node [right] at (4.74,6.32) {(3,4) $53.13^\circ$};</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="13"/>
+        <v>7.9209141336242288</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="14"/>
+        <v>10.561218844832306</v>
+      </c>
+      <c r="V28" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (3.6,4.8); \draw (0,0) -- (7.92,10.56);  \node [right] at (7.92,10.56) {(3,4) $53.13^\circ$};</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (2,3)</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>3.3282011773513749</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="5"/>
+        <v>4.9923017660270625</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (3.33,4.99); \draw (0,0) -- (4.44,6.66); </v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="7"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="8"/>
+        <v>4.4376015698018332</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="9"/>
+        <v>6.6564023547027498</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="10"/>
+        <v>56.309932474020215</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above] at (4.44,6.66) {$56.31^\circ$};</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (3.33,4.99); \draw (0,0) -- (4.62,6.92);  \node [right] at (4.62,6.92) {(2,3) $56.31^\circ$};</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="13"/>
+        <v>7.5652049721206254</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="14"/>
+        <v>11.347807458180938</v>
+      </c>
+      <c r="V29" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (3.33,4.99); \draw (0,0) -- (7.57,11.35);  \node [right] at (7.57,11.35) {(2,3) $56.31^\circ$};</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (4,6)</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="4"/>
+        <v>3.3282011773513749</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="5"/>
+        <v>4.9923017660270625</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (3.33,4.99); \draw (0,0) -- (4.44,6.66); </v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="7"/>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="8"/>
+        <v>4.4376015698018332</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="9"/>
+        <v>6.6564023547027498</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="10"/>
+        <v>56.309932474020215</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above] at (4.44,6.66) {$56.31^\circ$};</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (3.33,4.99); \draw (0,0) -- (4.62,6.92);  \node [right] at (4.62,6.92) {(4,6) $56.31^\circ$};</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="13"/>
+        <v>7.5652049721206254</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="14"/>
+        <v>11.347807458180938</v>
+      </c>
+      <c r="V30" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (3.33,4.99); \draw (0,0) -- (7.57,11.35);  \node [right] at (7.57,11.35) {(4,6) $56.31^\circ$};</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (3,5)</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>5.8309518948453007</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>3.0869745325651587</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="5"/>
+        <v>5.1449575542752646</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (3.09,5.14); \draw (0,0) -- (4.12,6.86); </v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="7"/>
+        <v>5.8309518948453007</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="8"/>
+        <v>4.1159660434202117</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="9"/>
+        <v>6.8599434057003528</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="10"/>
+        <v>59.036243467926482</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above] at (4.12,6.86) {$59.04^\circ$};</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (3.09,5.14); \draw (0,0) -- (4.5,7.5);  \node [right] at (4.5,7.5) {(3,5) $59.04^\circ$};</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="13"/>
+        <v>7.2171669627109427</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="14"/>
+        <v>12.028611604518238</v>
+      </c>
+      <c r="V31" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (3.09,5.14); \draw (0,0) -- (7.22,12.03);  \node [right] at (7.22,12.03) {(3,5) $59.04^\circ$};</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (1,2)</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>2.6832815729997477</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="5"/>
+        <v>5.3665631459994954</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (2.68,5.37); \draw (0,0) -- (3.58,7.16); </v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="7"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="8"/>
+        <v>3.5777087639996634</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="9"/>
+        <v>7.1554175279993268</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="10"/>
+        <v>63.43494882292201</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above] at (3.58,7.16) {$63.43^\circ$};</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (2.68,5.37); \draw (0,0) -- (3.14,6.29);  \node [right] at (3.14,6.29) {(1,2) $63.43^\circ$};</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="13"/>
+        <v>6.5662565162523405</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="14"/>
+        <v>13.132513032504681</v>
+      </c>
+      <c r="V32" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (2.68,5.37); \draw (0,0) -- (6.57,13.13);  \node [right] at (6.57,13.13) {(1,2) $63.43^\circ$};</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (2,4)</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="4"/>
+        <v>2.6832815729997477</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="5"/>
+        <v>5.3665631459994954</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (2.68,5.37); \draw (0,0) -- (3.58,7.16); </v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="7"/>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="8"/>
+        <v>3.5777087639996634</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="9"/>
+        <v>7.1554175279993268</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="10"/>
+        <v>63.43494882292201</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above] at (3.58,7.16) {$63.43^\circ$};</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (2.68,5.37); \draw (0,0) -- (3.14,6.29);  \node [right] at (3.14,6.29) {(2,4) $63.43^\circ$};</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="13"/>
+        <v>6.5662565162523405</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="14"/>
+        <v>13.132513032504681</v>
+      </c>
+      <c r="V33" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (2.68,5.37); \draw (0,0) -- (6.57,13.13);  \node [right] at (6.57,13.13) {(2,4) $63.43^\circ$};</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (3,6)</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>6.7082039324993694</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="4"/>
+        <v>2.6832815729997477</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="5"/>
+        <v>5.3665631459994954</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (2.68,5.37); \draw (0,0) -- (3.58,7.16); </v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="7"/>
+        <v>6.7082039324993694</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="8"/>
+        <v>3.5777087639996634</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="9"/>
+        <v>7.1554175279993268</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="10"/>
+        <v>63.43494882292201</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above] at (3.58,7.16) {$63.43^\circ$};</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (2.68,5.37); \draw (0,0) -- (3.14,6.29);  \node [right] at (3.14,6.29) {(3,6) $63.43^\circ$};</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="13"/>
+        <v>6.5662565162523405</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="14"/>
+        <v>13.132513032504681</v>
+      </c>
+      <c r="V34" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (2.68,5.37); \draw (0,0) -- (6.57,13.13);  \node [right] at (6.57,13.13) {(3,6) $63.43^\circ$};</v>
+      </c>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (2,5)</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>5.3851648071345037</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="4"/>
+        <v>2.2283440581246223</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="5"/>
+        <v>5.5708601453115563</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (2.23,5.57); \draw (0,0) -- (2.97,7.43); </v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="7"/>
+        <v>5.3851648071345037</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="8"/>
+        <v>2.9711254108328298</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="9"/>
+        <v>7.4278135270820753</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="10"/>
+        <v>68.198590513648185</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above] at (2.97,7.43) {$68.2^\circ$};</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (2.23,5.57); \draw (0,0) -- (2.93,7.33);  \node [right] at (2.93,7.33) {(2,5) $68.2^\circ$};</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="13"/>
+        <v>5.7289049281971813</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="14"/>
+        <v>14.322262320492953</v>
+      </c>
+      <c r="V35" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (2.23,5.57); \draw (0,0) -- (5.73,14.32);  \node [right] at (5.73,14.32) {(2,5) $68.2^\circ$};</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (1,3)</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="4"/>
+        <v>1.8973665961010275</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="5"/>
+        <v>5.6920997883030822</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (1.9,5.69); \draw (0,0) -- (2.53,7.59); </v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="7"/>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="8"/>
+        <v>2.5298221281347035</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="9"/>
+        <v>7.5894663844041101</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="10"/>
+        <v>71.56505117707799</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above left] at (2.53,7.59) {$71.57^\circ$};</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (1.9,5.69); \draw (0,0) -- (2.75,8.25);  \node [right] at (2.75,8.25) {(1,3) $71.57^\circ$};</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="13"/>
+        <v>5.0497501263116389</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="14"/>
+        <v>15.149250378934916</v>
+      </c>
+      <c r="V36" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (1.9,5.69); \draw (0,0) -- (5.05,15.15);  \node [right] at (5.05,15.15) {(1,3) $71.57^\circ$};</v>
+      </c>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (2,6)</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>6.324555320336759</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="4"/>
+        <v>1.8973665961010275</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="5"/>
+        <v>5.6920997883030822</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (1.9,5.69); \draw (0,0) -- (2.53,7.59); </v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="7"/>
+        <v>6.324555320336759</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="8"/>
+        <v>2.5298221281347035</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="9"/>
+        <v>7.5894663844041101</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="10"/>
+        <v>71.56505117707799</v>
+      </c>
+      <c r="P37" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above left] at (2.53,7.59) {$71.57^\circ$};</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" si="12"/>
+        <v>% \draw [-&gt;] (0,0) -- (1.9,5.69); \draw (0,0) -- (2.75,8.25);  \node [right] at (2.75,8.25) {(2,6) $71.57^\circ$};</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="13"/>
+        <v>5.0497501263116389</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="14"/>
+        <v>15.149250378934916</v>
+      </c>
+      <c r="V37" t="str">
+        <f t="shared" si="15"/>
+        <v>% \draw [-&gt;] (0,0) -- (1.9,5.69); \draw (0,0) -- (5.05,15.15);  \node [right] at (5.05,15.15) {(2,6) $71.57^\circ$};</v>
+      </c>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (1,4)</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>4.1231056256176606</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="4"/>
+        <v>1.4552137502179978</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="5"/>
+        <v>5.8208550008719913</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (1.46,5.82); \draw (0,0) -- (1.94,7.76); </v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="7"/>
+        <v>4.1231056256176606</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="8"/>
+        <v>1.9402850002906638</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="9"/>
+        <v>7.761140001162655</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="10"/>
+        <v>75.963756532073532</v>
+      </c>
+      <c r="P38" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above left] at (1.94,7.76) {$75.96^\circ$};</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (1.46,5.82); \draw (0,0) -- (2.44,9.78);  \node [right] at (2.44,9.78) {(1,4) $75.96^\circ$};</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="13"/>
+        <v>4.0495230558595381</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="14"/>
+        <v>16.198092223438152</v>
+      </c>
+      <c r="V38" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (1.46,5.82); \draw (0,0) -- (4.05,16.2);  \node [right] at (4.05,16.2) {(1,4) $75.96^\circ$};</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (1,5)</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="3"/>
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>1.1766968108291043</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="5"/>
+        <v>5.8834840541455211</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (1.18,5.88); \draw (0,0) -- (1.57,7.84); </v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="7"/>
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="8"/>
+        <v>1.5689290811054724</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="9"/>
+        <v>7.8446454055273618</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="10"/>
+        <v>78.690067525979799</v>
+      </c>
+      <c r="P39" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above left] at (1.57,7.84) {$78.69^\circ$};</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (1.18,5.88); \draw (0,0) -- (2.2,11);  \node [right] at (2.2,11) {(1,5) $78.69^\circ$};</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="13"/>
+        <v>3.3645154688971397</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="14"/>
+        <v>16.822577344485698</v>
+      </c>
+      <c r="V39" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (1.18,5.88); \draw (0,0) -- (3.36,16.82);  \node [right] at (3.36,16.82) {(1,5) $78.69^\circ$};</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="2"/>
+        <v>\draw [-&gt;] (1,6)</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>6.0827625302982193</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>0.98639392383214375</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="5"/>
+        <v>5.9183635429928625</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">\draw [-&gt;] (0,0) -- (0.99,5.92); \draw (0,0) -- (1.32,7.89); </v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="7"/>
+        <v>6.0827625302982193</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="8"/>
+        <v>1.3151918984428583</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="9"/>
+        <v>7.89115139065715</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="10"/>
+        <v>80.537677791974389</v>
+      </c>
+      <c r="P40" t="str">
+        <f t="shared" si="11"/>
+        <v>\node [above left] at (1.32,7.89) {$80.54^\circ$};</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" si="12"/>
+        <v>\draw [-&gt;] (0,0) -- (0.99,5.92); \draw (0,0) -- (2,12);  \node [right] at (2,12) {(1,6) $80.54^\circ$};</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="13"/>
+        <v>2.8719490680273401</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="14"/>
+        <v>17.231694408164039</v>
+      </c>
+      <c r="V40" t="str">
+        <f t="shared" si="15"/>
+        <v>\draw [-&gt;] (0,0) -- (0.99,5.92); \draw (0,0) -- (2.87,17.23);  \node [right] at (2.87,17.23) {(1,6) $80.54^\circ$};</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B2:Q37">
+    <sortCondition ref="O2:O37"/>
+    <sortCondition ref="C2:C37"/>
+    <sortCondition ref="D2:D37"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed images and added friction examples
</commit_message>
<xml_diff>
--- a/ABIP.xlsx
+++ b/ABIP.xlsx
@@ -4005,8 +4005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4037,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>2+IF(MOD(A2,5)=0,2,0)</f>
+        <f t="shared" ref="B2:B33" si="0">2+IF(MOD(A2,5)=0,2,0)</f>
         <v>4</v>
       </c>
       <c r="C2">
@@ -4047,649 +4047,649 @@
         <v>35</v>
       </c>
       <c r="F2" t="str">
-        <f>CONCATENATE("\draw (",C2,",",F$1,") -- (",C2,",",F$1+2*$B2,");",IF($A2/10=TRUNC($A2/10),CONCATENATE(" \node [above,right] at (",C2,",",F$1+2*$B2,") {",$A2/10,"};"),""))</f>
-        <v>\draw (5,26) -- (5,34); \node [above,right] at (5,34) {0};</v>
+        <f>CONCATENATE("\draw (",C2,",",F$1,") -- (",C2,",",F$1+2*$B2,");",IF($A2/10=TRUNC($A2/10),CONCATENATE(" \node [above right] at (",C2,",",F$1+2*$B2,") {",$A2/10,"};"),""))</f>
+        <v>\draw (5,26) -- (5,34); \node [above right] at (5,34) {0};</v>
       </c>
       <c r="G2" t="str">
-        <f>CONCATENATE("\draw (",D2,",",G$1,") -- (",D2,",",G$1-$B2,");",IF($B2=4,CONCATENATE(" \node [above,right] at (",D2,",",G$1-$B2,") {",$A2,"};"),""))</f>
-        <v>\draw (35,23) -- (35,19); \node [above,right] at (35,19) {0};</v>
+        <f>CONCATENATE("\draw (",D2,",",G$1,") -- (",D2,",",G$1-$B2,");",IF($B2=4,CONCATENATE(" \node [below right] at (",D2,",",G$1-$B2,") {",$A2,"};"),""))</f>
+        <v>\draw (35,23) -- (35,19); \node [below right] at (35,19) {0};</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A33" si="1">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3">
-        <f>2+IF(MOD(A3,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C3">
-        <f>C2+1.9</f>
+        <f t="shared" ref="C3:C33" si="2">C2+1.9</f>
         <v>6.9</v>
       </c>
       <c r="D3">
-        <f>D2+1</f>
+        <f t="shared" ref="D3:D12" si="3">D2+1</f>
         <v>36</v>
       </c>
       <c r="F3" t="str">
-        <f>CONCATENATE("\draw (",C3,",",F$1,") -- (",C3,",",F$1+2*$B3,");",IF($A3/10=TRUNC($A3/10),CONCATENATE(" \node [above,right] at (",C3,",",F$1+2*$B3,") {",$A3/10,"};"),""))</f>
+        <f t="shared" ref="F3:F33" si="4">CONCATENATE("\draw (",C3,",",F$1,") -- (",C3,",",F$1+2*$B3,");",IF($A3/10=TRUNC($A3/10),CONCATENATE(" \node [above right] at (",C3,",",F$1+2*$B3,") {",$A3/10,"};"),""))</f>
         <v>\draw (6.9,26) -- (6.9,30);</v>
       </c>
       <c r="G3" t="str">
-        <f>CONCATENATE("\draw (",D3,",",G$1,") -- (",D3,",",G$1-$B3,");",IF($B3=4,CONCATENATE(" \node [above,right] at (",D3,",",G$1-$B3,") {",$A3,"};"),""))</f>
+        <f t="shared" ref="G3:G12" si="5">CONCATENATE("\draw (",D3,",",G$1,") -- (",D3,",",G$1-$B3,");",IF($B3=4,CONCATENATE(" \node [below right] at (",D3,",",G$1-$B3,") {",$A3,"};"),""))</f>
         <v>\draw (36,23) -- (36,21);</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>A3+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="B4">
-        <f>2+IF(MOD(A4,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C4">
-        <f>C3+1.9</f>
+        <f t="shared" si="2"/>
         <v>8.8000000000000007</v>
       </c>
       <c r="D4">
-        <f>D3+1</f>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="F4" t="str">
-        <f>CONCATENATE("\draw (",C4,",",F$1,") -- (",C4,",",F$1+2*$B4,");",IF($A4/10=TRUNC($A4/10),CONCATENATE(" \node [above,right] at (",C4,",",F$1+2*$B4,") {",$A4/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (8.8,26) -- (8.8,30);</v>
       </c>
       <c r="G4" t="str">
-        <f>CONCATENATE("\draw (",D4,",",G$1,") -- (",D4,",",G$1-$B4,");",IF($B4=4,CONCATENATE(" \node [above,right] at (",D4,",",G$1-$B4,") {",$A4,"};"),""))</f>
+        <f t="shared" si="5"/>
         <v>\draw (37,23) -- (37,21);</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>A4+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B5">
-        <f>2+IF(MOD(A5,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C5">
-        <f>C4+1.9</f>
+        <f t="shared" si="2"/>
         <v>10.700000000000001</v>
       </c>
       <c r="D5">
-        <f>D4+1</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="F5" t="str">
-        <f>CONCATENATE("\draw (",C5,",",F$1,") -- (",C5,",",F$1+2*$B5,");",IF($A5/10=TRUNC($A5/10),CONCATENATE(" \node [above,right] at (",C5,",",F$1+2*$B5,") {",$A5/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (10.7,26) -- (10.7,30);</v>
       </c>
       <c r="G5" t="str">
-        <f>CONCATENATE("\draw (",D5,",",G$1,") -- (",D5,",",G$1-$B5,");",IF($B5=4,CONCATENATE(" \node [above,right] at (",D5,",",G$1-$B5,") {",$A5,"};"),""))</f>
+        <f t="shared" si="5"/>
         <v>\draw (38,23) -- (38,21);</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>A5+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6">
-        <f>2+IF(MOD(A6,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C6">
-        <f>C5+1.9</f>
+        <f t="shared" si="2"/>
         <v>12.600000000000001</v>
       </c>
       <c r="D6">
-        <f>D5+1</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="F6" t="str">
-        <f>CONCATENATE("\draw (",C6,",",F$1,") -- (",C6,",",F$1+2*$B6,");",IF($A6/10=TRUNC($A6/10),CONCATENATE(" \node [above,right] at (",C6,",",F$1+2*$B6,") {",$A6/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (12.6,26) -- (12.6,30);</v>
       </c>
       <c r="G6" t="str">
-        <f>CONCATENATE("\draw (",D6,",",G$1,") -- (",D6,",",G$1-$B6,");",IF($B6=4,CONCATENATE(" \node [above,right] at (",D6,",",G$1-$B6,") {",$A6,"};"),""))</f>
+        <f t="shared" si="5"/>
         <v>\draw (39,23) -- (39,21);</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>A6+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7">
-        <f>2+IF(MOD(A7,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C7">
-        <f>C6+1.9</f>
+        <f t="shared" si="2"/>
         <v>14.500000000000002</v>
       </c>
       <c r="D7">
-        <f>D6+1</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="F7" t="str">
-        <f>CONCATENATE("\draw (",C7,",",F$1,") -- (",C7,",",F$1+2*$B7,");",IF($A7/10=TRUNC($A7/10),CONCATENATE(" \node [above,right] at (",C7,",",F$1+2*$B7,") {",$A7/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (14.5,26) -- (14.5,34);</v>
       </c>
       <c r="G7" t="str">
-        <f>CONCATENATE("\draw (",D7,",",G$1,") -- (",D7,",",G$1-$B7,");",IF($B7=4,CONCATENATE(" \node [above,right] at (",D7,",",G$1-$B7,") {",$A7,"};"),""))</f>
-        <v>\draw (40,23) -- (40,19); \node [above,right] at (40,19) {5};</v>
+        <f t="shared" si="5"/>
+        <v>\draw (40,23) -- (40,19); \node [below right] at (40,19) {5};</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>A7+1</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8">
-        <f>2+IF(MOD(A8,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C8">
-        <f>C7+1.9</f>
+        <f t="shared" si="2"/>
         <v>16.400000000000002</v>
       </c>
       <c r="D8">
-        <f>D7+1</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="F8" t="str">
-        <f>CONCATENATE("\draw (",C8,",",F$1,") -- (",C8,",",F$1+2*$B8,");",IF($A8/10=TRUNC($A8/10),CONCATENATE(" \node [above,right] at (",C8,",",F$1+2*$B8,") {",$A8/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (16.4,26) -- (16.4,30);</v>
       </c>
       <c r="G8" t="str">
-        <f>CONCATENATE("\draw (",D8,",",G$1,") -- (",D8,",",G$1-$B8,");",IF($B8=4,CONCATENATE(" \node [above,right] at (",D8,",",G$1-$B8,") {",$A8,"};"),""))</f>
+        <f t="shared" si="5"/>
         <v>\draw (41,23) -- (41,21);</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>A8+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9">
-        <f>2+IF(MOD(A9,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C9">
-        <f>C8+1.9</f>
+        <f t="shared" si="2"/>
         <v>18.3</v>
       </c>
       <c r="D9">
-        <f>D8+1</f>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="F9" t="str">
-        <f>CONCATENATE("\draw (",C9,",",F$1,") -- (",C9,",",F$1+2*$B9,");",IF($A9/10=TRUNC($A9/10),CONCATENATE(" \node [above,right] at (",C9,",",F$1+2*$B9,") {",$A9/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (18.3,26) -- (18.3,30);</v>
       </c>
       <c r="G9" t="str">
-        <f>CONCATENATE("\draw (",D9,",",G$1,") -- (",D9,",",G$1-$B9,");",IF($B9=4,CONCATENATE(" \node [above,right] at (",D9,",",G$1-$B9,") {",$A9,"};"),""))</f>
+        <f t="shared" si="5"/>
         <v>\draw (42,23) -- (42,21);</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>A9+1</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10">
-        <f>2+IF(MOD(A10,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C10">
-        <f>C9+1.9</f>
+        <f t="shared" si="2"/>
         <v>20.2</v>
       </c>
       <c r="D10">
-        <f>D9+1</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="F10" t="str">
-        <f>CONCATENATE("\draw (",C10,",",F$1,") -- (",C10,",",F$1+2*$B10,");",IF($A10/10=TRUNC($A10/10),CONCATENATE(" \node [above,right] at (",C10,",",F$1+2*$B10,") {",$A10/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (20.2,26) -- (20.2,30);</v>
       </c>
       <c r="G10" t="str">
-        <f>CONCATENATE("\draw (",D10,",",G$1,") -- (",D10,",",G$1-$B10,");",IF($B10=4,CONCATENATE(" \node [above,right] at (",D10,",",G$1-$B10,") {",$A10,"};"),""))</f>
+        <f t="shared" si="5"/>
         <v>\draw (43,23) -- (43,21);</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>A10+1</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B11">
-        <f>2+IF(MOD(A11,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C11">
-        <f>C10+1.9</f>
+        <f t="shared" si="2"/>
         <v>22.099999999999998</v>
       </c>
       <c r="D11">
-        <f>D10+1</f>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="F11" t="str">
-        <f>CONCATENATE("\draw (",C11,",",F$1,") -- (",C11,",",F$1+2*$B11,");",IF($A11/10=TRUNC($A11/10),CONCATENATE(" \node [above,right] at (",C11,",",F$1+2*$B11,") {",$A11/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (22.1,26) -- (22.1,30);</v>
       </c>
       <c r="G11" t="str">
-        <f>CONCATENATE("\draw (",D11,",",G$1,") -- (",D11,",",G$1-$B11,");",IF($B11=4,CONCATENATE(" \node [above,right] at (",D11,",",G$1-$B11,") {",$A11,"};"),""))</f>
+        <f t="shared" si="5"/>
         <v>\draw (44,23) -- (44,21);</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>A11+1</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12">
-        <f>2+IF(MOD(A12,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C12">
-        <f>C11+1.9</f>
+        <f t="shared" si="2"/>
         <v>23.999999999999996</v>
       </c>
       <c r="D12">
-        <f>D11+1</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="F12" t="str">
-        <f>CONCATENATE("\draw (",C12,",",F$1,") -- (",C12,",",F$1+2*$B12,");",IF($A12/10=TRUNC($A12/10),CONCATENATE(" \node [above,right] at (",C12,",",F$1+2*$B12,") {",$A12/10,"};"),""))</f>
-        <v>\draw (24,26) -- (24,34); \node [above,right] at (24,34) {1};</v>
+        <f t="shared" si="4"/>
+        <v>\draw (24,26) -- (24,34); \node [above right] at (24,34) {1};</v>
       </c>
       <c r="G12" t="str">
-        <f>CONCATENATE("\draw (",D12,",",G$1,") -- (",D12,",",G$1-$B12,");",IF($B12=4,CONCATENATE(" \node [above,right] at (",D12,",",G$1-$B12,") {",$A12,"};"),""))</f>
-        <v>\draw (45,23) -- (45,19); \node [above,right] at (45,19) {10};</v>
+        <f t="shared" si="5"/>
+        <v>\draw (45,23) -- (45,19); \node [below right] at (45,19) {10};</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>A12+1</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B13">
-        <f>2+IF(MOD(A13,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C13">
-        <f>C12+1.9</f>
+        <f t="shared" si="2"/>
         <v>25.899999999999995</v>
       </c>
       <c r="F13" t="str">
-        <f>CONCATENATE("\draw (",C13,",",F$1,") -- (",C13,",",F$1+2*$B13,");",IF($A13/10=TRUNC($A13/10),CONCATENATE(" \node [above,right] at (",C13,",",F$1+2*$B13,") {",$A13/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (25.9,26) -- (25.9,30);</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>A13+1</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B14">
-        <f>2+IF(MOD(A14,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C14">
-        <f>C13+1.9</f>
+        <f t="shared" si="2"/>
         <v>27.799999999999994</v>
       </c>
       <c r="F14" t="str">
-        <f>CONCATENATE("\draw (",C14,",",F$1,") -- (",C14,",",F$1+2*$B14,");",IF($A14/10=TRUNC($A14/10),CONCATENATE(" \node [above,right] at (",C14,",",F$1+2*$B14,") {",$A14/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (27.8,26) -- (27.8,30);</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>A14+1</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B15">
-        <f>2+IF(MOD(A15,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C15">
-        <f>C14+1.9</f>
+        <f t="shared" si="2"/>
         <v>29.699999999999992</v>
       </c>
       <c r="F15" t="str">
-        <f>CONCATENATE("\draw (",C15,",",F$1,") -- (",C15,",",F$1+2*$B15,");",IF($A15/10=TRUNC($A15/10),CONCATENATE(" \node [above,right] at (",C15,",",F$1+2*$B15,") {",$A15/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (29.7,26) -- (29.7,30);</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>A15+1</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B16">
-        <f>2+IF(MOD(A16,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C16">
-        <f>C15+1.9</f>
+        <f t="shared" si="2"/>
         <v>31.599999999999991</v>
       </c>
       <c r="F16" t="str">
-        <f>CONCATENATE("\draw (",C16,",",F$1,") -- (",C16,",",F$1+2*$B16,");",IF($A16/10=TRUNC($A16/10),CONCATENATE(" \node [above,right] at (",C16,",",F$1+2*$B16,") {",$A16/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (31.6,26) -- (31.6,30);</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>A16+1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B17">
-        <f>2+IF(MOD(A17,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C17">
-        <f>C16+1.9</f>
+        <f t="shared" si="2"/>
         <v>33.499999999999993</v>
       </c>
       <c r="F17" t="str">
-        <f>CONCATENATE("\draw (",C17,",",F$1,") -- (",C17,",",F$1+2*$B17,");",IF($A17/10=TRUNC($A17/10),CONCATENATE(" \node [above,right] at (",C17,",",F$1+2*$B17,") {",$A17/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (33.5,26) -- (33.5,34);</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>A17+1</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B18">
-        <f>2+IF(MOD(A18,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C18">
-        <f>C17+1.9</f>
+        <f t="shared" si="2"/>
         <v>35.399999999999991</v>
       </c>
       <c r="F18" t="str">
-        <f>CONCATENATE("\draw (",C18,",",F$1,") -- (",C18,",",F$1+2*$B18,");",IF($A18/10=TRUNC($A18/10),CONCATENATE(" \node [above,right] at (",C18,",",F$1+2*$B18,") {",$A18/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (35.4,26) -- (35.4,30);</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>A18+1</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B19">
-        <f>2+IF(MOD(A19,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C19">
-        <f>C18+1.9</f>
+        <f t="shared" si="2"/>
         <v>37.29999999999999</v>
       </c>
       <c r="F19" t="str">
-        <f>CONCATENATE("\draw (",C19,",",F$1,") -- (",C19,",",F$1+2*$B19,");",IF($A19/10=TRUNC($A19/10),CONCATENATE(" \node [above,right] at (",C19,",",F$1+2*$B19,") {",$A19/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (37.3,26) -- (37.3,30);</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>A19+1</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B20">
-        <f>2+IF(MOD(A20,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C20">
-        <f>C19+1.9</f>
+        <f t="shared" si="2"/>
         <v>39.199999999999989</v>
       </c>
       <c r="F20" t="str">
-        <f>CONCATENATE("\draw (",C20,",",F$1,") -- (",C20,",",F$1+2*$B20,");",IF($A20/10=TRUNC($A20/10),CONCATENATE(" \node [above,right] at (",C20,",",F$1+2*$B20,") {",$A20/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (39.2,26) -- (39.2,30);</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>A20+1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B21">
-        <f>2+IF(MOD(A21,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C21">
-        <f>C20+1.9</f>
+        <f t="shared" si="2"/>
         <v>41.099999999999987</v>
       </c>
       <c r="F21" t="str">
-        <f>CONCATENATE("\draw (",C21,",",F$1,") -- (",C21,",",F$1+2*$B21,");",IF($A21/10=TRUNC($A21/10),CONCATENATE(" \node [above,right] at (",C21,",",F$1+2*$B21,") {",$A21/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (41.1,26) -- (41.1,30);</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>A21+1</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B22">
-        <f>2+IF(MOD(A22,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C22">
-        <f>C21+1.9</f>
+        <f t="shared" si="2"/>
         <v>42.999999999999986</v>
       </c>
       <c r="F22" t="str">
-        <f>CONCATENATE("\draw (",C22,",",F$1,") -- (",C22,",",F$1+2*$B22,");",IF($A22/10=TRUNC($A22/10),CONCATENATE(" \node [above,right] at (",C22,",",F$1+2*$B22,") {",$A22/10,"};"),""))</f>
-        <v>\draw (43,26) -- (43,34); \node [above,right] at (43,34) {2};</v>
+        <f t="shared" si="4"/>
+        <v>\draw (43,26) -- (43,34); \node [above right] at (43,34) {2};</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>A22+1</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B23">
-        <f>2+IF(MOD(A23,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C23">
-        <f>C22+1.9</f>
+        <f t="shared" si="2"/>
         <v>44.899999999999984</v>
       </c>
       <c r="F23" t="str">
-        <f>CONCATENATE("\draw (",C23,",",F$1,") -- (",C23,",",F$1+2*$B23,");",IF($A23/10=TRUNC($A23/10),CONCATENATE(" \node [above,right] at (",C23,",",F$1+2*$B23,") {",$A23/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (44.9,26) -- (44.9,30);</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>A23+1</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B24">
-        <f>2+IF(MOD(A24,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C24">
-        <f>C23+1.9</f>
+        <f t="shared" si="2"/>
         <v>46.799999999999983</v>
       </c>
       <c r="F24" t="str">
-        <f>CONCATENATE("\draw (",C24,",",F$1,") -- (",C24,",",F$1+2*$B24,");",IF($A24/10=TRUNC($A24/10),CONCATENATE(" \node [above,right] at (",C24,",",F$1+2*$B24,") {",$A24/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (46.8,26) -- (46.8,30);</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>A24+1</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B25">
-        <f>2+IF(MOD(A25,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C25">
-        <f>C24+1.9</f>
+        <f t="shared" si="2"/>
         <v>48.699999999999982</v>
       </c>
       <c r="F25" t="str">
-        <f>CONCATENATE("\draw (",C25,",",F$1,") -- (",C25,",",F$1+2*$B25,");",IF($A25/10=TRUNC($A25/10),CONCATENATE(" \node [above,right] at (",C25,",",F$1+2*$B25,") {",$A25/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (48.7,26) -- (48.7,30);</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>A25+1</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B26">
-        <f>2+IF(MOD(A26,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C26">
-        <f>C25+1.9</f>
+        <f t="shared" si="2"/>
         <v>50.59999999999998</v>
       </c>
       <c r="F26" t="str">
-        <f>CONCATENATE("\draw (",C26,",",F$1,") -- (",C26,",",F$1+2*$B26,");",IF($A26/10=TRUNC($A26/10),CONCATENATE(" \node [above,right] at (",C26,",",F$1+2*$B26,") {",$A26/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (50.6,26) -- (50.6,30);</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>A26+1</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B27">
-        <f>2+IF(MOD(A27,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C27">
-        <f>C26+1.9</f>
+        <f t="shared" si="2"/>
         <v>52.499999999999979</v>
       </c>
       <c r="F27" t="str">
-        <f>CONCATENATE("\draw (",C27,",",F$1,") -- (",C27,",",F$1+2*$B27,");",IF($A27/10=TRUNC($A27/10),CONCATENATE(" \node [above,right] at (",C27,",",F$1+2*$B27,") {",$A27/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (52.5,26) -- (52.5,34);</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>A27+1</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B28">
-        <f>2+IF(MOD(A28,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C28">
-        <f>C27+1.9</f>
+        <f t="shared" si="2"/>
         <v>54.399999999999977</v>
       </c>
       <c r="F28" t="str">
-        <f>CONCATENATE("\draw (",C28,",",F$1,") -- (",C28,",",F$1+2*$B28,");",IF($A28/10=TRUNC($A28/10),CONCATENATE(" \node [above,right] at (",C28,",",F$1+2*$B28,") {",$A28/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (54.4,26) -- (54.4,30);</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>A28+1</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B29">
-        <f>2+IF(MOD(A29,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C29">
-        <f>C28+1.9</f>
+        <f t="shared" si="2"/>
         <v>56.299999999999976</v>
       </c>
       <c r="F29" t="str">
-        <f>CONCATENATE("\draw (",C29,",",F$1,") -- (",C29,",",F$1+2*$B29,");",IF($A29/10=TRUNC($A29/10),CONCATENATE(" \node [above,right] at (",C29,",",F$1+2*$B29,") {",$A29/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (56.3,26) -- (56.3,30);</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>A29+1</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B30">
-        <f>2+IF(MOD(A30,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C30">
-        <f>C29+1.9</f>
+        <f t="shared" si="2"/>
         <v>58.199999999999974</v>
       </c>
       <c r="F30" t="str">
-        <f>CONCATENATE("\draw (",C30,",",F$1,") -- (",C30,",",F$1+2*$B30,");",IF($A30/10=TRUNC($A30/10),CONCATENATE(" \node [above,right] at (",C30,",",F$1+2*$B30,") {",$A30/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (58.2,26) -- (58.2,30);</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>A30+1</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B31">
-        <f>2+IF(MOD(A31,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C31">
-        <f>C30+1.9</f>
+        <f t="shared" si="2"/>
         <v>60.099999999999973</v>
       </c>
       <c r="F31" t="str">
-        <f>CONCATENATE("\draw (",C31,",",F$1,") -- (",C31,",",F$1+2*$B31,");",IF($A31/10=TRUNC($A31/10),CONCATENATE(" \node [above,right] at (",C31,",",F$1+2*$B31,") {",$A31/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (60.1,26) -- (60.1,30);</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>A31+1</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B32">
-        <f>2+IF(MOD(A32,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C32">
-        <f>C31+1.9</f>
+        <f t="shared" si="2"/>
         <v>61.999999999999972</v>
       </c>
       <c r="F32" t="str">
-        <f>CONCATENATE("\draw (",C32,",",F$1,") -- (",C32,",",F$1+2*$B32,");",IF($A32/10=TRUNC($A32/10),CONCATENATE(" \node [above,right] at (",C32,",",F$1+2*$B32,") {",$A32/10,"};"),""))</f>
-        <v>\draw (62,26) -- (62,34); \node [above,right] at (62,34) {3};</v>
+        <f t="shared" si="4"/>
+        <v>\draw (62,26) -- (62,34); \node [above right] at (62,34) {3};</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>A32+1</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B33">
-        <f>2+IF(MOD(A33,5)=0,2,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C33">
-        <f>C32+1.9</f>
+        <f t="shared" si="2"/>
         <v>63.89999999999997</v>
       </c>
       <c r="F33" t="str">
-        <f>CONCATENATE("\draw (",C33,",",F$1,") -- (",C33,",",F$1+2*$B33,");",IF($A33/10=TRUNC($A33/10),CONCATENATE(" \node [above,right] at (",C33,",",F$1+2*$B33,") {",$A33/10,"};"),""))</f>
+        <f t="shared" si="4"/>
         <v>\draw (63.9,26) -- (63.9,30);</v>
       </c>
     </row>

</xml_diff>